<commit_message>
Removed capacitor (C45) guess for link
</commit_message>
<xml_diff>
--- a/AQ32_v2/AQ32_v2_BOM.xlsx
+++ b/AQ32_v2/AQ32_v2_BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="AQ32_v2_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="208">
   <si>
     <t>Qty</t>
   </si>
@@ -630,9 +630,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/SN74AHC1G86DCKR/296-8750-1-ND/373813</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/C1206C476M8PACTU/399-5508-1-ND/1950686</t>
   </si>
   <si>
     <t>MPU6000</t>
@@ -1499,7 +1496,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -2272,9 +2269,6 @@
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
-      <c r="H26" t="s">
-        <v>205</v>
-      </c>
       <c r="I26" t="s">
         <v>14</v>
       </c>
@@ -2497,10 +2491,10 @@
         <v>104</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>103</v>
@@ -2803,7 +2797,7 @@
         <v>108</v>
       </c>
       <c r="G44" s="3">
-        <f>A44*F44</f>
+        <f t="shared" ref="G44:G49" si="1">A44*F44</f>
         <v>0</v>
       </c>
       <c r="H44" t="s">
@@ -2830,7 +2824,7 @@
         <v>120</v>
       </c>
       <c r="G45" s="3">
-        <f>A45*F45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H45" t="s">
@@ -2857,7 +2851,7 @@
         <v>116</v>
       </c>
       <c r="G46" s="3">
-        <f>A46*F46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H46" t="s">
@@ -2884,7 +2878,7 @@
         <v>113</v>
       </c>
       <c r="G47" s="3">
-        <f>A47*F47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H47" t="s">
@@ -2908,7 +2902,7 @@
         <v>7</v>
       </c>
       <c r="G48" s="3">
-        <f>A48*F48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H48" t="s">
@@ -2923,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>19</v>
@@ -2935,7 +2929,7 @@
         <v>21</v>
       </c>
       <c r="G49" s="3">
-        <f>A49*F49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H49" t="s">

</xml_diff>

<commit_message>
Ala42 added HMC5983 support, remapped receiver/motor lines to match v1 board, moved mag to avoid interference, made space for standoffs by moving uSD conenctor, made power lines thicker
</commit_message>
<xml_diff>
--- a/AQ32_v2/AQ32_v2_BOM.xlsx
+++ b/AQ32_v2/AQ32_v2_BOM.xlsx
@@ -442,12 +442,6 @@
     <t>C18</t>
   </si>
   <si>
-    <t>R37, R38</t>
-  </si>
-  <si>
-    <t>R45, R54, R58</t>
-  </si>
-  <si>
     <t>2x08</t>
   </si>
   <si>
@@ -470,6 +464,12 @@
   </si>
   <si>
     <t>STM32F407VGT6</t>
+  </si>
+  <si>
+    <t>R54, R58</t>
+  </si>
+  <si>
+    <t>R37, R38, R45</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1321,8 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -2083,7 +2083,7 @@
         <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>101</v>
@@ -2175,16 +2175,16 @@
         <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>116</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>120</v>
@@ -2267,10 +2267,10 @@
         <v>95</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>95</v>
@@ -2379,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>139</v>
@@ -2402,13 +2402,13 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
ala42 added blocking cap for uSD (C10), updated silkscreen to v2.0.2, replaced R54 to C54 (2.2uF) for F4 compatibility
</commit_message>
<xml_diff>
--- a/AQ32_v2/AQ32_v2_BOM.xlsx
+++ b/AQ32_v2/AQ32_v2_BOM.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ted\SkyDrive\Development\FlightControlBoards\AQ32_v2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2550" windowWidth="21285" windowHeight="6300"/>
+    <workbookView xWindow="-12" yWindow="2556" windowWidth="12240" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="AQ32_v2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="146">
   <si>
     <t>Qty</t>
   </si>
@@ -151,18 +156,12 @@
     <t>2.2uF</t>
   </si>
   <si>
-    <t>C41</t>
-  </si>
-  <si>
     <t>220R</t>
   </si>
   <si>
     <t>R62</t>
   </si>
   <si>
-    <t>220uF</t>
-  </si>
-  <si>
     <t>C42</t>
   </si>
   <si>
@@ -172,12 +171,6 @@
     <t>R26, R35</t>
   </si>
   <si>
-    <t>22uH</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>30V</t>
   </si>
   <si>
@@ -205,15 +198,6 @@
     <t>47uF</t>
   </si>
   <si>
-    <t>C-USC1206</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>C44</t>
-  </si>
-  <si>
     <t>4k7</t>
   </si>
   <si>
@@ -283,9 +267,6 @@
     <t>LED2</t>
   </si>
   <si>
-    <t>HMC5883LSMD</t>
-  </si>
-  <si>
     <t>16LPCC</t>
   </si>
   <si>
@@ -382,18 +363,9 @@
     <t>S1</t>
   </si>
   <si>
-    <t>USBOLD</t>
-  </si>
-  <si>
-    <t>USB-MINIB-OLD</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
-    <t>USB Connectors</t>
-  </si>
-  <si>
     <t>USD-SOCKETNEW</t>
   </si>
   <si>
@@ -418,27 +390,18 @@
     <t>MPU-6000</t>
   </si>
   <si>
-    <t>C4, C6, C8, C12, C15, C17, C22, C29, C39, C40, C45</t>
-  </si>
-  <si>
     <t>R1, R2, R8, R52, R60, R64</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>JP5, JP6</t>
-  </si>
-  <si>
     <t>MPU-6000 6DOF IMU</t>
   </si>
   <si>
     <t>Do Not Install</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>C18</t>
   </si>
   <si>
@@ -466,10 +429,34 @@
     <t>STM32F407VGT6</t>
   </si>
   <si>
-    <t>R54, R58</t>
-  </si>
-  <si>
     <t>R37, R38, R45</t>
+  </si>
+  <si>
+    <t>HMC5983-TR</t>
+  </si>
+  <si>
+    <t>JP5</t>
+  </si>
+  <si>
+    <t>C5, C44</t>
+  </si>
+  <si>
+    <t>CONN USB MINI B R/A SMD</t>
+  </si>
+  <si>
+    <t>USB-M26FTR</t>
+  </si>
+  <si>
+    <t>Mini USB Connector</t>
+  </si>
+  <si>
+    <t>C41, C54</t>
+  </si>
+  <si>
+    <t>R39, R40, R58</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C8, C10, C12, C15, C17, C22, C29, C39, C40, C45</t>
   </si>
 </sst>
 </file>
@@ -960,7 +947,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -974,6 +961,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1027,6 +1020,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1074,7 +1070,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1109,7 +1105,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1318,33 +1314,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -1359,15 +1355,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1382,7 +1378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1390,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -1405,7 +1401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1422,13 +1418,13 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -1451,7 +1447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1474,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1482,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -1491,13 +1487,13 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1505,7 +1501,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1514,13 +1510,13 @@
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1528,7 +1524,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1543,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -1560,21 +1556,21 @@
         <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1589,7 +1585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1612,7 +1608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1620,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1635,7 +1631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1658,7 +1654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1681,7 +1677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1704,7 +1700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1727,7 +1723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1750,7 +1746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1773,15 +1769,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -1796,7 +1792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1804,22 +1800,22 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1827,68 +1823,68 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
+      </c>
+      <c r="E24" s="1">
+        <v>805</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1896,114 +1892,114 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="1">
-        <v>805</v>
+        <v>69</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="1">
-        <v>805</v>
+        <v>74</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2011,68 +2007,68 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2080,45 +2076,45 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D33" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2126,22 +2122,22 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2149,45 +2145,45 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2195,22 +2191,22 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2218,114 +2214,114 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D39" t="s">
-        <v>125</v>
+        <v>87</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="G39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G40" t="s">
+      <c r="E40" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="F40" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2333,68 +2329,68 @@
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="5">
-        <v>2</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2402,71 +2398,26 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>145</v>
+        <v>97</v>
+      </c>
+      <c r="D47" t="s">
+        <v>98</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>47</v>
-      </c>
-      <c r="B48" s="2">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" t="s">
-        <v>138</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G48" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>48</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" t="s">
-        <v>106</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>